<commit_message>
FEAT: divide input output Matertial data
</commit_message>
<xml_diff>
--- a/input/Material/MaterialData.xlsx
+++ b/input/Material/MaterialData.xlsx
@@ -7,7 +7,10 @@
     <workbookView xWindow="360" yWindow="30" windowWidth="25755" windowHeight="11595" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="input" sheetId="1" r:id="rId1"/>
+    <sheet name="output" sheetId="2" r:id="rId2"/>
+    <sheet name="Example input data" sheetId="3" r:id="rId3"/>
+    <sheet name="Example output data" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="152511"/>
@@ -15,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
   <si>
     <t>Material_Name</t>
   </si>
@@ -105,13 +108,189 @@
   </si>
   <si>
     <t>0.00053</t>
+  </si>
+  <si>
+    <t>FlowName</t>
+  </si>
+  <si>
+    <t>Natural Gas</t>
+  </si>
+  <si>
+    <t>입력 규칮</t>
+  </si>
+  <si>
+    <t>입력 규칙</t>
+  </si>
+  <si>
+    <t>입력 규칙_x000D_</t>
+  </si>
+  <si>
+    <t>입력 규칙_x000D__x000D_</t>
+  </si>
+  <si>
+    <t>입력 규칙_x000D__x000D__x000D_</t>
+  </si>
+  <si>
+    <t>입력 규칙_x000D__x000D__x000D_ ㅁㄴㅇ</t>
+  </si>
+  <si>
+    <t>ㅁㄴㅇ</t>
+  </si>
+  <si>
+    <t>입력 규칙_x000D__x000D__x000D_ㅁㄴㅇ</t>
+  </si>
+  <si>
+    <t>입력 규칙_x000D__x000D__x000D_ㅁㄴㅇ_x000D_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">사용 메뉴얼
+- 이곳은 product 물질의 데이터를 저장하는 곳입니다.
+- product가 여러개일 경우를 대비해 각 product의 flow name를 명시해주시길 바랍니다.
+- example output data sheet를 참고해 시트를 작성해주시길 바랍니다.
+- 물질은 위에서부터 아래까지 빈칸없이 작성해주셔야 합니다.
+- </t>
+  </si>
+  <si>
+    <t xml:space="preserve">사용 메뉴얼_x000D_
+- 이곳은 product 물질의 데이터를 저장하는 곳입니다.
+- product가 여러개일 경우를 대비해 각 product의 flow name를 명시해주시길 바랍니다.
+- example output data sheet를 참고해 시트를 작성해주시길 바랍니다.
+- 물질은 위에서부터 아래까지 빈칸없이 작성해주셔야 합니다.
+- </t>
+  </si>
+  <si>
+    <t xml:space="preserve">사용 메뉴얼_x000D_
+- 이곳은 product 물질의 데이터를 저장하는 곳입니다.
+- product가 여러개일 경우를 대비해 각 product의 flow name를 명시해주시길 바랍니다.
+- example output data sheet를 참고해 시트를 작성해주시길 바랍니다.
+- 물질은 위에서부터 아래까지 빈칸없이 작성해주셔야 합니다.
+- </t>
+  </si>
+  <si>
+    <t xml:space="preserve">사용 메뉴얼_x000D_
+- 이곳은 product 물질의 데이터를 저장하는 곳입니다.
+- product가 여러개일 경우를 대비해 각 product의 flow name를 명시해주시길 바랍니다
+- example output data sheet를 참고해 시트를 작성해주시길 바랍니다.
+- 물질은 위에서부터 아래까지 빈칸없이 작성해주셔야 합니다.
+- </t>
+  </si>
+  <si>
+    <t xml:space="preserve">사용 메뉴얼_x000D_
+- 이곳은 product 물질의 데이터를 저장하는 곳입니다.
+- product가 여러개일 경우를 대비해 각 product의 flow name를 명시해주시길 바랍니다. 만약 product 물질이 하나더라도 FlowName은 작성하셔야 합니다.
+- example output data sheet를 참고해 시트를 작성해주시길 바랍니다.
+- 물질은 위에서부터 아래까지 빈칸없이 작성해주셔야 합니다.
+- </t>
+  </si>
+  <si>
+    <t>CO3</t>
+  </si>
+  <si>
+    <t>H3</t>
+  </si>
+  <si>
+    <t>O3</t>
+  </si>
+  <si>
+    <t>H3O</t>
+  </si>
+  <si>
+    <t>CO4</t>
+  </si>
+  <si>
+    <t>H4</t>
+  </si>
+  <si>
+    <t>O4</t>
+  </si>
+  <si>
+    <t>H4O</t>
+  </si>
+  <si>
+    <t>CO5</t>
+  </si>
+  <si>
+    <t>H5</t>
+  </si>
+  <si>
+    <t>O5</t>
+  </si>
+  <si>
+    <t>H5O</t>
+  </si>
+  <si>
+    <t>44.02</t>
+  </si>
+  <si>
+    <t>18.016</t>
+  </si>
+  <si>
+    <t>44.03</t>
+  </si>
+  <si>
+    <t>18.017</t>
+  </si>
+  <si>
+    <t>44.04</t>
+  </si>
+  <si>
+    <t>18.018</t>
+  </si>
+  <si>
+    <t>0.0559</t>
+  </si>
+  <si>
+    <t>0.00054</t>
+  </si>
+  <si>
+    <t>0.0560</t>
+  </si>
+  <si>
+    <t>0.00055</t>
+  </si>
+  <si>
+    <t>0.0561</t>
+  </si>
+  <si>
+    <t>0.00056</t>
+  </si>
+  <si>
+    <t>사용 메뉴얼</t>
+  </si>
+  <si>
+    <t>- 이곳은 product 물질의 데이터를 저장하는 곳입니다.</t>
+  </si>
+  <si>
+    <t>- product가 여러개일 경우를 대비해 각 product의 flow name를 명시해주시길 바랍니다. 만약 product 물질이 하나더라도 FlowName은 작성하셔야 합니다.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>- example output data sheet를 참고해 시트를 작성해주시길 바랍니다.</t>
+  </si>
+  <si>
+    <t>- 물질은 위에서부터 아래까지 빈칸없이 작성해주셔야 합니다.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- </t>
+  </si>
+  <si>
+    <t xml:space="preserve">사용 메뉴얼_x000D_
+- 이곳은 input 물질의 데이터를 저장하는 곳입니다.
+- example input data sheet를 참고해 시트를 작성해주시길 바랍니다. 
+- 물질은 위에서부터 아래까지 빈칸없이 작성해주셔야 합니다. 
+- 
+- </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="64" formatCode="@"/>
+  </numFmts>
   <fonts count="22">
     <font>
       <sz val="11.0"/>
@@ -443,7 +622,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -562,6 +741,156 @@
         <color theme="4"/>
       </bottom>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFAAAAAA"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFAAAAAA"/>
+      </top>
+      <bottom/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FFAAAAAA"/>
+      </top>
+      <bottom/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFAAAAAA"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFAAAAAA"/>
+      </top>
+      <bottom/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFAAAAAA"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFAAAAAA"/>
+      </right>
+      <top/>
+      <bottom/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFAAAAAA"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFAAAAAA"/>
+      </bottom>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFAAAAAA"/>
+      </bottom>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFAAAAAA"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFAAAAAA"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0">
@@ -712,7 +1041,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -743,6 +1072,172 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="64" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="64" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="64" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="64" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="64" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="64" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="64" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="64" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="64" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="64" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="64" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="64" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="64" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="64" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="64" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="64" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="64" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="64" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="64" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1825,10 +2320,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:Y40"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="F2" sqref="F2:N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333000" defaultRowHeight="15.000000" customHeight="1"/>
@@ -1840,14 +2335,34 @@
     <col min="5" max="16384" style="1" width="8.88000011" customWidth="1" outlineLevel="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.000000" customHeight="1">
+    <row r="1" spans="1:25" ht="16.000000" customHeight="1">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
-    </row>
-    <row r="2" spans="1:5" ht="16.000000" customHeight="1">
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+    </row>
+    <row r="2" spans="1:25" ht="16.000000" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="4" t="s">
         <v>0</v>
@@ -1859,8 +2374,30 @@
         <v>2</v>
       </c>
       <c r="E2" s="2"/>
-    </row>
-    <row r="3" spans="1:5" ht="16.000000" customHeight="1">
+      <c r="F2" s="67" t="s">
+        <v>77</v>
+      </c>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="59"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="60"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+    </row>
+    <row r="3" spans="1:25" ht="16.000000" customHeight="1">
       <c r="A3" s="2"/>
       <c r="B3" s="4" t="s">
         <v>3</v>
@@ -1872,8 +2409,28 @@
         <v>5</v>
       </c>
       <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:5" ht="16.000000" customHeight="1">
+      <c r="F3" s="61"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="62"/>
+      <c r="I3" s="62"/>
+      <c r="J3" s="62"/>
+      <c r="K3" s="62"/>
+      <c r="L3" s="62"/>
+      <c r="M3" s="62"/>
+      <c r="N3" s="63"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
+    </row>
+    <row r="4" spans="1:25" ht="16.000000" customHeight="1">
       <c r="A4" s="2"/>
       <c r="B4" s="4" t="s">
         <v>6</v>
@@ -1885,280 +2442,1027 @@
         <v>5</v>
       </c>
       <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" ht="16.000000" customHeight="1">
+      <c r="F4" s="61" t="s">
+        <v>71</v>
+      </c>
+      <c r="G4" s="62"/>
+      <c r="H4" s="62"/>
+      <c r="I4" s="62"/>
+      <c r="J4" s="62"/>
+      <c r="K4" s="62"/>
+      <c r="L4" s="62"/>
+      <c r="M4" s="62"/>
+      <c r="N4" s="63"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="2"/>
+    </row>
+    <row r="5" spans="1:25" ht="16.000000" customHeight="1">
       <c r="A5" s="2"/>
       <c r="B5" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C5" s="12">
-        <v>28.014</v>
+        <v>32</v>
       </c>
       <c r="D5" s="12">
-        <v>2</v>
+        <v>0.08</v>
       </c>
       <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" ht="16.000000" customHeight="1">
+      <c r="F5" s="61"/>
+      <c r="G5" s="62"/>
+      <c r="H5" s="62"/>
+      <c r="I5" s="62"/>
+      <c r="J5" s="62"/>
+      <c r="K5" s="62"/>
+      <c r="L5" s="62"/>
+      <c r="M5" s="62"/>
+      <c r="N5" s="63"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="2"/>
+    </row>
+    <row r="6" spans="1:25" ht="16.000000" customHeight="1">
       <c r="A6" s="2"/>
-      <c r="B6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="12">
-        <v>32</v>
-      </c>
-      <c r="D6" s="12">
-        <v>0.08</v>
+      <c r="B6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" ht="16.000000" customHeight="1">
+      <c r="F6" s="61" t="s">
+        <v>72</v>
+      </c>
+      <c r="G6" s="62"/>
+      <c r="H6" s="62"/>
+      <c r="I6" s="62"/>
+      <c r="J6" s="62"/>
+      <c r="K6" s="62"/>
+      <c r="L6" s="62"/>
+      <c r="M6" s="62"/>
+      <c r="N6" s="63"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+      <c r="V6" s="2"/>
+      <c r="W6" s="2"/>
+      <c r="X6" s="2"/>
+      <c r="Y6" s="2"/>
+    </row>
+    <row r="7" spans="1:25" ht="16.000000" customHeight="1">
       <c r="A7" s="2"/>
-      <c r="B7" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>29</v>
-      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
       <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" ht="16.000000" customHeight="1">
+      <c r="F7" s="61" t="s">
+        <v>73</v>
+      </c>
+      <c r="G7" s="62"/>
+      <c r="H7" s="62"/>
+      <c r="I7" s="62"/>
+      <c r="J7" s="62"/>
+      <c r="K7" s="62"/>
+      <c r="L7" s="62"/>
+      <c r="M7" s="62"/>
+      <c r="N7" s="63"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2"/>
+      <c r="V7" s="2"/>
+      <c r="W7" s="2"/>
+      <c r="X7" s="2"/>
+      <c r="Y7" s="2"/>
+    </row>
+    <row r="8" spans="1:25" ht="16.000000" customHeight="1">
       <c r="A8" s="2"/>
-      <c r="B8" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="13">
-        <v>16.04</v>
-      </c>
-      <c r="D8" s="13">
-        <v>0.325</v>
-      </c>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
       <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" ht="16.000000" customHeight="1">
+      <c r="F8" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="G8" s="62"/>
+      <c r="H8" s="62"/>
+      <c r="I8" s="62"/>
+      <c r="J8" s="62"/>
+      <c r="K8" s="62"/>
+      <c r="L8" s="62"/>
+      <c r="M8" s="62"/>
+      <c r="N8" s="63"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2"/>
+      <c r="V8" s="2"/>
+      <c r="W8" s="2"/>
+      <c r="X8" s="2"/>
+      <c r="Y8" s="2"/>
+    </row>
+    <row r="9" spans="1:25" ht="16.000000" customHeight="1">
       <c r="A9" s="2"/>
-      <c r="B9" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="13">
-        <v>30.07</v>
-      </c>
-      <c r="D9" s="13">
-        <v>0.325</v>
-      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
       <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:5" ht="16.000000" customHeight="1">
+      <c r="F9" s="61"/>
+      <c r="G9" s="62"/>
+      <c r="H9" s="62"/>
+      <c r="I9" s="62"/>
+      <c r="J9" s="62"/>
+      <c r="K9" s="62"/>
+      <c r="L9" s="62"/>
+      <c r="M9" s="62"/>
+      <c r="N9" s="63"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
+      <c r="V9" s="2"/>
+      <c r="W9" s="2"/>
+      <c r="X9" s="2"/>
+      <c r="Y9" s="2"/>
+    </row>
+    <row r="10" spans="1:25" ht="16.000000" customHeight="1">
       <c r="A10" s="2"/>
-      <c r="B10" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="13">
-        <v>44.1</v>
-      </c>
-      <c r="D10" s="13">
-        <v>0.325</v>
-      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
       <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:5" ht="16.000000" customHeight="1">
+      <c r="F10" s="61" t="s">
+        <v>75</v>
+      </c>
+      <c r="G10" s="62"/>
+      <c r="H10" s="62"/>
+      <c r="I10" s="62"/>
+      <c r="J10" s="62"/>
+      <c r="K10" s="62"/>
+      <c r="L10" s="62"/>
+      <c r="M10" s="62"/>
+      <c r="N10" s="63"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
+      <c r="V10" s="2"/>
+      <c r="W10" s="2"/>
+      <c r="X10" s="2"/>
+      <c r="Y10" s="2"/>
+    </row>
+    <row r="11" spans="1:25" ht="16.000000" customHeight="1">
       <c r="A11" s="2"/>
-      <c r="B11" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="13">
-        <v>58.12</v>
-      </c>
-      <c r="D11" s="13">
-        <v>0.325</v>
-      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
       <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:5" ht="16.000000" customHeight="1">
+      <c r="F11" s="61"/>
+      <c r="G11" s="62"/>
+      <c r="H11" s="62"/>
+      <c r="I11" s="62"/>
+      <c r="J11" s="62"/>
+      <c r="K11" s="62"/>
+      <c r="L11" s="62"/>
+      <c r="M11" s="62"/>
+      <c r="N11" s="63"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2"/>
+      <c r="V11" s="2"/>
+      <c r="W11" s="2"/>
+      <c r="X11" s="2"/>
+      <c r="Y11" s="2"/>
+    </row>
+    <row r="12" spans="1:25" ht="16.000000" customHeight="1">
       <c r="A12" s="2"/>
-      <c r="B12" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="13">
-        <v>72.15</v>
-      </c>
-      <c r="D12" s="13">
-        <v>0.325</v>
-      </c>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
       <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="B13" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="13">
-        <v>86.18</v>
-      </c>
-      <c r="D13" s="13">
-        <v>0.325</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="B14" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="13">
-        <v>100.2</v>
-      </c>
-      <c r="D14" s="13">
-        <v>0.325</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="B15" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="13">
-        <v>114.23</v>
-      </c>
-      <c r="D15" s="13">
-        <v>0.325</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="B16" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="13">
-        <v>128.26</v>
-      </c>
-      <c r="D16" s="13">
-        <v>0.325</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4">
-      <c r="B17" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="13">
-        <v>142.29</v>
-      </c>
-      <c r="D17" s="13">
-        <v>0.325</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4">
-      <c r="B18" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="13">
-        <v>156.31</v>
-      </c>
-      <c r="D18" s="13">
-        <v>0.325</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4">
-      <c r="B19" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="13">
-        <v>170.34</v>
-      </c>
-      <c r="D19" s="13">
-        <v>0.325</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4">
-      <c r="B20" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" s="13">
-        <v>184.37</v>
-      </c>
-      <c r="D20" s="13">
-        <v>0.325</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4">
-      <c r="B21" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" s="13">
-        <v>198.39</v>
-      </c>
-      <c r="D21" s="13">
-        <v>0.325</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4">
-      <c r="B22" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" s="13">
-        <v>212.42</v>
-      </c>
-      <c r="D22" s="13">
-        <v>0.325</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4">
-      <c r="B23" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C23" s="13">
-        <v>226.45</v>
-      </c>
-      <c r="D23" s="13">
-        <v>0.325</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4">
-      <c r="B24" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24" s="13">
-        <v>240.48</v>
-      </c>
-      <c r="D24" s="13">
-        <v>0.325</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4">
-      <c r="B25" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C25" s="13">
-        <v>254.5</v>
-      </c>
-      <c r="D25" s="13">
-        <v>0.325</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4">
-      <c r="B26" s="14"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-    </row>
-    <row r="27" spans="2:4">
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-    </row>
-    <row r="28" spans="2:4">
-      <c r="B28" s="14"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-    </row>
-    <row r="29" spans="2:4">
-      <c r="B29" s="14"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-    </row>
-    <row r="30" spans="2:4">
-      <c r="B30" s="14"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
+      <c r="F12" s="61" t="s">
+        <v>76</v>
+      </c>
+      <c r="G12" s="62"/>
+      <c r="H12" s="62"/>
+      <c r="I12" s="62"/>
+      <c r="J12" s="62"/>
+      <c r="K12" s="62"/>
+      <c r="L12" s="62"/>
+      <c r="M12" s="62"/>
+      <c r="N12" s="63"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2"/>
+      <c r="V12" s="2"/>
+      <c r="W12" s="2"/>
+      <c r="X12" s="2"/>
+      <c r="Y12" s="2"/>
+    </row>
+    <row r="13" spans="1:25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="64"/>
+      <c r="G13" s="65"/>
+      <c r="H13" s="65"/>
+      <c r="I13" s="65"/>
+      <c r="J13" s="65"/>
+      <c r="K13" s="65"/>
+      <c r="L13" s="65"/>
+      <c r="M13" s="65"/>
+      <c r="N13" s="66"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2"/>
+      <c r="V13" s="2"/>
+      <c r="W13" s="2"/>
+      <c r="X13" s="2"/>
+      <c r="Y13" s="2"/>
+    </row>
+    <row r="14" spans="1:25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2"/>
+      <c r="T14" s="2"/>
+      <c r="U14" s="2"/>
+      <c r="V14" s="2"/>
+      <c r="W14" s="2"/>
+      <c r="X14" s="2"/>
+      <c r="Y14" s="2"/>
+    </row>
+    <row r="15" spans="1:25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2"/>
+      <c r="T15" s="2"/>
+      <c r="U15" s="2"/>
+      <c r="V15" s="2"/>
+      <c r="W15" s="2"/>
+      <c r="X15" s="2"/>
+      <c r="Y15" s="2"/>
+    </row>
+    <row r="16" spans="1:25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
+      <c r="T16" s="2"/>
+      <c r="U16" s="2"/>
+      <c r="V16" s="2"/>
+      <c r="W16" s="2"/>
+      <c r="X16" s="2"/>
+      <c r="Y16" s="2"/>
+    </row>
+    <row r="17" spans="1:25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="2"/>
+      <c r="S17" s="2"/>
+      <c r="T17" s="2"/>
+      <c r="U17" s="2"/>
+      <c r="V17" s="2"/>
+      <c r="W17" s="2"/>
+      <c r="X17" s="2"/>
+      <c r="Y17" s="2"/>
+    </row>
+    <row r="18" spans="1:25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
+      <c r="S18" s="2"/>
+      <c r="T18" s="2"/>
+      <c r="U18" s="2"/>
+      <c r="V18" s="2"/>
+      <c r="W18" s="2"/>
+      <c r="X18" s="2"/>
+      <c r="Y18" s="2"/>
+    </row>
+    <row r="19" spans="1:25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="2"/>
+      <c r="S19" s="2"/>
+      <c r="T19" s="2"/>
+      <c r="U19" s="2"/>
+      <c r="V19" s="2"/>
+      <c r="W19" s="2"/>
+      <c r="X19" s="2"/>
+      <c r="Y19" s="2"/>
+    </row>
+    <row r="20" spans="1:25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2"/>
+      <c r="R20" s="2"/>
+      <c r="S20" s="2"/>
+      <c r="T20" s="2"/>
+      <c r="U20" s="2"/>
+      <c r="V20" s="2"/>
+      <c r="W20" s="2"/>
+      <c r="X20" s="2"/>
+      <c r="Y20" s="2"/>
+    </row>
+    <row r="21" spans="1:25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2"/>
+      <c r="R21" s="2"/>
+      <c r="S21" s="2"/>
+      <c r="T21" s="2"/>
+      <c r="U21" s="2"/>
+      <c r="V21" s="2"/>
+      <c r="W21" s="2"/>
+      <c r="X21" s="2"/>
+      <c r="Y21" s="2"/>
+    </row>
+    <row r="22" spans="1:25">
+      <c r="A22" s="2"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2"/>
+      <c r="R22" s="2"/>
+      <c r="S22" s="2"/>
+      <c r="T22" s="2"/>
+      <c r="U22" s="2"/>
+      <c r="V22" s="2"/>
+      <c r="W22" s="2"/>
+      <c r="X22" s="2"/>
+      <c r="Y22" s="2"/>
+    </row>
+    <row r="23" spans="1:25">
+      <c r="A23" s="2"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="2"/>
+      <c r="S23" s="2"/>
+      <c r="T23" s="2"/>
+      <c r="U23" s="2"/>
+      <c r="V23" s="2"/>
+      <c r="W23" s="2"/>
+      <c r="X23" s="2"/>
+      <c r="Y23" s="2"/>
+    </row>
+    <row r="24" spans="1:25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
+      <c r="R24" s="2"/>
+      <c r="S24" s="2"/>
+      <c r="T24" s="2"/>
+      <c r="U24" s="2"/>
+      <c r="V24" s="2"/>
+      <c r="W24" s="2"/>
+      <c r="X24" s="2"/>
+      <c r="Y24" s="2"/>
+    </row>
+    <row r="25" spans="1:25">
+      <c r="A25" s="2"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="2"/>
+      <c r="R25" s="2"/>
+      <c r="S25" s="2"/>
+      <c r="T25" s="2"/>
+      <c r="U25" s="2"/>
+      <c r="V25" s="2"/>
+      <c r="W25" s="2"/>
+      <c r="X25" s="2"/>
+      <c r="Y25" s="2"/>
+    </row>
+    <row r="26" spans="1:25">
+      <c r="A26" s="2"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="2"/>
+      <c r="R26" s="2"/>
+      <c r="S26" s="2"/>
+      <c r="T26" s="2"/>
+      <c r="U26" s="2"/>
+      <c r="V26" s="2"/>
+      <c r="W26" s="2"/>
+      <c r="X26" s="2"/>
+      <c r="Y26" s="2"/>
+    </row>
+    <row r="27" spans="1:25">
+      <c r="A27" s="2"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2"/>
+      <c r="R27" s="2"/>
+      <c r="S27" s="2"/>
+      <c r="T27" s="2"/>
+      <c r="U27" s="2"/>
+      <c r="V27" s="2"/>
+      <c r="W27" s="2"/>
+      <c r="X27" s="2"/>
+      <c r="Y27" s="2"/>
+    </row>
+    <row r="28" spans="1:25">
+      <c r="A28" s="2"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
+      <c r="P28" s="2"/>
+      <c r="Q28" s="2"/>
+      <c r="R28" s="2"/>
+      <c r="S28" s="2"/>
+      <c r="T28" s="2"/>
+      <c r="U28" s="2"/>
+      <c r="V28" s="2"/>
+      <c r="W28" s="2"/>
+      <c r="X28" s="2"/>
+      <c r="Y28" s="2"/>
+    </row>
+    <row r="29" spans="1:25">
+      <c r="A29" s="2"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
+      <c r="P29" s="2"/>
+      <c r="Q29" s="2"/>
+      <c r="R29" s="2"/>
+      <c r="S29" s="2"/>
+      <c r="T29" s="2"/>
+      <c r="U29" s="2"/>
+      <c r="V29" s="2"/>
+      <c r="W29" s="2"/>
+      <c r="X29" s="2"/>
+      <c r="Y29" s="2"/>
+    </row>
+    <row r="30" spans="1:25">
+      <c r="A30" s="2"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+      <c r="P30" s="2"/>
+      <c r="Q30" s="2"/>
+      <c r="R30" s="2"/>
+      <c r="S30" s="2"/>
+      <c r="T30" s="2"/>
+      <c r="U30" s="2"/>
+      <c r="V30" s="2"/>
+      <c r="W30" s="2"/>
+      <c r="X30" s="2"/>
+      <c r="Y30" s="2"/>
+    </row>
+    <row r="31" spans="1:25">
+      <c r="A31" s="2"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+      <c r="P31" s="2"/>
+      <c r="Q31" s="2"/>
+      <c r="R31" s="2"/>
+      <c r="S31" s="2"/>
+      <c r="T31" s="2"/>
+      <c r="U31" s="2"/>
+      <c r="V31" s="2"/>
+      <c r="W31" s="2"/>
+      <c r="X31" s="2"/>
+      <c r="Y31" s="2"/>
+    </row>
+    <row r="32" spans="1:25">
+      <c r="A32" s="2"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
+      <c r="O32" s="2"/>
+      <c r="P32" s="2"/>
+      <c r="Q32" s="2"/>
+      <c r="R32" s="2"/>
+      <c r="S32" s="2"/>
+      <c r="T32" s="2"/>
+      <c r="U32" s="2"/>
+      <c r="V32" s="2"/>
+      <c r="W32" s="2"/>
+      <c r="X32" s="2"/>
+      <c r="Y32" s="2"/>
+    </row>
+    <row r="33" spans="1:25">
+      <c r="A33" s="2"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+      <c r="O33" s="2"/>
+      <c r="P33" s="2"/>
+      <c r="Q33" s="2"/>
+      <c r="R33" s="2"/>
+      <c r="S33" s="2"/>
+      <c r="T33" s="2"/>
+      <c r="U33" s="2"/>
+      <c r="V33" s="2"/>
+      <c r="W33" s="2"/>
+      <c r="X33" s="2"/>
+      <c r="Y33" s="2"/>
+    </row>
+    <row r="34" spans="1:25">
+      <c r="A34" s="2"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+      <c r="O34" s="2"/>
+      <c r="P34" s="2"/>
+      <c r="Q34" s="2"/>
+      <c r="R34" s="2"/>
+      <c r="S34" s="2"/>
+      <c r="T34" s="2"/>
+      <c r="U34" s="2"/>
+      <c r="V34" s="2"/>
+      <c r="W34" s="2"/>
+      <c r="X34" s="2"/>
+      <c r="Y34" s="2"/>
+    </row>
+    <row r="35" spans="1:25">
+      <c r="A35" s="2"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
+      <c r="O35" s="2"/>
+      <c r="P35" s="2"/>
+      <c r="Q35" s="2"/>
+      <c r="R35" s="2"/>
+      <c r="S35" s="2"/>
+      <c r="T35" s="2"/>
+      <c r="U35" s="2"/>
+      <c r="V35" s="2"/>
+      <c r="W35" s="2"/>
+      <c r="X35" s="2"/>
+      <c r="Y35" s="2"/>
+    </row>
+    <row r="36" spans="1:25">
+      <c r="A36" s="2"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+      <c r="O36" s="2"/>
+      <c r="P36" s="2"/>
+      <c r="Q36" s="2"/>
+      <c r="R36" s="2"/>
+      <c r="S36" s="2"/>
+      <c r="T36" s="2"/>
+      <c r="U36" s="2"/>
+      <c r="V36" s="2"/>
+      <c r="W36" s="2"/>
+      <c r="X36" s="2"/>
+      <c r="Y36" s="2"/>
+    </row>
+    <row r="37" spans="1:25">
+      <c r="A37" s="2"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
+      <c r="O37" s="2"/>
+      <c r="P37" s="2"/>
+      <c r="Q37" s="2"/>
+      <c r="R37" s="2"/>
+      <c r="S37" s="2"/>
+      <c r="T37" s="2"/>
+      <c r="U37" s="2"/>
+      <c r="V37" s="2"/>
+      <c r="W37" s="2"/>
+      <c r="X37" s="2"/>
+      <c r="Y37" s="2"/>
+    </row>
+    <row r="38" spans="1:25">
+      <c r="A38" s="2"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
+      <c r="M38" s="2"/>
+      <c r="N38" s="2"/>
+      <c r="O38" s="2"/>
+      <c r="P38" s="2"/>
+      <c r="Q38" s="2"/>
+      <c r="R38" s="2"/>
+      <c r="S38" s="2"/>
+      <c r="T38" s="2"/>
+      <c r="U38" s="2"/>
+      <c r="V38" s="2"/>
+      <c r="W38" s="2"/>
+      <c r="X38" s="2"/>
+      <c r="Y38" s="2"/>
+    </row>
+    <row r="39" spans="1:25">
+      <c r="A39" s="2"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
+      <c r="M39" s="2"/>
+      <c r="N39" s="2"/>
+      <c r="O39" s="2"/>
+      <c r="P39" s="2"/>
+      <c r="Q39" s="2"/>
+      <c r="R39" s="2"/>
+      <c r="S39" s="2"/>
+      <c r="T39" s="2"/>
+      <c r="U39" s="2"/>
+      <c r="V39" s="2"/>
+      <c r="W39" s="2"/>
+      <c r="X39" s="2"/>
+      <c r="Y39" s="2"/>
+    </row>
+    <row r="40" spans="1:25">
+      <c r="A40" s="2"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
+      <c r="O40" s="2"/>
+      <c r="P40" s="2"/>
+      <c r="Q40" s="2"/>
+      <c r="R40" s="2"/>
+      <c r="S40" s="2"/>
+      <c r="T40" s="2"/>
+      <c r="U40" s="2"/>
+      <c r="V40" s="2"/>
+      <c r="W40" s="2"/>
+      <c r="X40" s="2"/>
+      <c r="Y40" s="2"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F2:N13"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.70" right="0.70" top="0.75" bottom="0.75" header="0.30" footer="0.30"/>
   <pageSetup paperSize="1" orientation="portrait"/>
@@ -2166,4 +3470,783 @@
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B1:N20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.200000"/>
+  <cols>
+    <col min="2" max="2" width="21.12999916" customWidth="1" outlineLevel="0"/>
+    <col min="3" max="3" width="28.12999916" customWidth="1" outlineLevel="0"/>
+    <col min="4" max="4" width="20.75499916" customWidth="1" outlineLevel="0"/>
+    <col min="5" max="5" width="22.50499916" customWidth="1" outlineLevel="0"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:14">
+      <c r="B2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14">
+      <c r="B3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="13">
+        <v>16.04</v>
+      </c>
+      <c r="D3" s="13">
+        <v>0.325</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="31"/>
+      <c r="N3" s="32"/>
+    </row>
+    <row r="4" spans="2:14">
+      <c r="B4" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="13">
+        <v>30.07</v>
+      </c>
+      <c r="D4" s="13">
+        <v>0.325</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="33"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="34"/>
+      <c r="K4" s="34"/>
+      <c r="L4" s="34"/>
+      <c r="M4" s="34"/>
+      <c r="N4" s="35"/>
+    </row>
+    <row r="5" spans="2:14">
+      <c r="B5" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="13">
+        <v>44.1</v>
+      </c>
+      <c r="D5" s="13">
+        <v>0.325</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="33"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="34"/>
+      <c r="K5" s="34"/>
+      <c r="L5" s="34"/>
+      <c r="M5" s="34"/>
+      <c r="N5" s="35"/>
+    </row>
+    <row r="6" spans="2:14">
+      <c r="B6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="13">
+        <v>58.12</v>
+      </c>
+      <c r="D6" s="13">
+        <v>0.325</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="33"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="34"/>
+      <c r="K6" s="34"/>
+      <c r="L6" s="34"/>
+      <c r="M6" s="34"/>
+      <c r="N6" s="35"/>
+    </row>
+    <row r="7" spans="2:14">
+      <c r="B7" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="13">
+        <v>72.15</v>
+      </c>
+      <c r="D7" s="13">
+        <v>0.325</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="33"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="34"/>
+      <c r="K7" s="34"/>
+      <c r="L7" s="34"/>
+      <c r="M7" s="34"/>
+      <c r="N7" s="35"/>
+    </row>
+    <row r="8" spans="2:14">
+      <c r="B8" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="13">
+        <v>86.18</v>
+      </c>
+      <c r="D8" s="13">
+        <v>0.325</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="33"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="34"/>
+      <c r="K8" s="34"/>
+      <c r="L8" s="34"/>
+      <c r="M8" s="34"/>
+      <c r="N8" s="35"/>
+    </row>
+    <row r="9" spans="2:14">
+      <c r="B9" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="13">
+        <v>100.2</v>
+      </c>
+      <c r="D9" s="13">
+        <v>0.325</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="33"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="34"/>
+      <c r="I9" s="34"/>
+      <c r="J9" s="34"/>
+      <c r="K9" s="34"/>
+      <c r="L9" s="34"/>
+      <c r="M9" s="34"/>
+      <c r="N9" s="35"/>
+    </row>
+    <row r="10" spans="2:14">
+      <c r="B10" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="13">
+        <v>114.23</v>
+      </c>
+      <c r="D10" s="13">
+        <v>0.325</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="33"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
+      <c r="I10" s="34"/>
+      <c r="J10" s="34"/>
+      <c r="K10" s="34"/>
+      <c r="L10" s="34"/>
+      <c r="M10" s="34"/>
+      <c r="N10" s="35"/>
+    </row>
+    <row r="11" spans="2:14">
+      <c r="B11" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="13">
+        <v>128.26</v>
+      </c>
+      <c r="D11" s="13">
+        <v>0.325</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" s="33"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="34"/>
+      <c r="J11" s="34"/>
+      <c r="K11" s="34"/>
+      <c r="L11" s="34"/>
+      <c r="M11" s="34"/>
+      <c r="N11" s="35"/>
+    </row>
+    <row r="12" spans="2:14">
+      <c r="B12" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="13">
+        <v>142.29</v>
+      </c>
+      <c r="D12" s="13">
+        <v>0.325</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="33"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="34"/>
+      <c r="L12" s="34"/>
+      <c r="M12" s="34"/>
+      <c r="N12" s="35"/>
+    </row>
+    <row r="13" spans="2:14">
+      <c r="B13" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="13">
+        <v>156.31</v>
+      </c>
+      <c r="D13" s="13">
+        <v>0.325</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="33"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="34"/>
+      <c r="J13" s="34"/>
+      <c r="K13" s="34"/>
+      <c r="L13" s="34"/>
+      <c r="M13" s="34"/>
+      <c r="N13" s="35"/>
+    </row>
+    <row r="14" spans="2:14">
+      <c r="B14" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="13">
+        <v>170.34</v>
+      </c>
+      <c r="D14" s="13">
+        <v>0.325</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" s="33"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="34"/>
+      <c r="L14" s="34"/>
+      <c r="M14" s="34"/>
+      <c r="N14" s="35"/>
+    </row>
+    <row r="15" spans="2:14">
+      <c r="B15" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="13">
+        <v>184.37</v>
+      </c>
+      <c r="D15" s="13">
+        <v>0.325</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15" s="36"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="37"/>
+      <c r="J15" s="37"/>
+      <c r="K15" s="37"/>
+      <c r="L15" s="37"/>
+      <c r="M15" s="37"/>
+      <c r="N15" s="38"/>
+    </row>
+    <row r="16" spans="2:14">
+      <c r="B16" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="13">
+        <v>198.39</v>
+      </c>
+      <c r="D16" s="13">
+        <v>0.325</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="F16" s="39"/>
+    </row>
+    <row r="17" spans="2:7">
+      <c r="B17" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="13">
+        <v>212.42</v>
+      </c>
+      <c r="D17" s="13">
+        <v>0.325</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7">
+      <c r="B18" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="13">
+        <v>226.45</v>
+      </c>
+      <c r="D18" s="13">
+        <v>0.325</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="G18" s="16"/>
+    </row>
+    <row r="19" spans="2:7">
+      <c r="B19" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="13">
+        <v>240.48</v>
+      </c>
+      <c r="D19" s="13">
+        <v>0.325</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7">
+      <c r="B20" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="13">
+        <v>254.5</v>
+      </c>
+      <c r="D20" s="13">
+        <v>0.325</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F3:N15"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.70" right="0.70" top="0.75" bottom="0.75" header="0.30" footer="0.30"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B2:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.200000"/>
+  <cols>
+    <col min="2" max="2" width="15.38000011" customWidth="1" outlineLevel="0"/>
+    <col min="3" max="3" width="24.12999916" customWidth="1" outlineLevel="0"/>
+    <col min="4" max="4" width="23.00499916" customWidth="1" outlineLevel="0"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4">
+      <c r="B2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4">
+      <c r="B3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4">
+      <c r="B4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="12">
+        <v>2.016</v>
+      </c>
+      <c r="D4" s="12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4">
+      <c r="B5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="12">
+        <v>32</v>
+      </c>
+      <c r="D5" s="12">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4">
+      <c r="B6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.70" right="0.70" top="0.75" bottom="0.75" header="0.30" footer="0.30"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B2:E20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.200000"/>
+  <cols>
+    <col min="2" max="2" width="15.38000011" customWidth="1" outlineLevel="0"/>
+    <col min="3" max="3" width="24.12999916" customWidth="1" outlineLevel="0"/>
+    <col min="4" max="4" width="23.00499916" customWidth="1" outlineLevel="0"/>
+    <col min="5" max="5" width="12.13000011" customWidth="1" outlineLevel="0"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5">
+      <c r="B2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5">
+      <c r="B3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="13">
+        <v>16.04</v>
+      </c>
+      <c r="D3" s="13">
+        <v>0.325</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5">
+      <c r="B4" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="13">
+        <v>30.07</v>
+      </c>
+      <c r="D4" s="13">
+        <v>0.325</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5">
+      <c r="B5" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="13">
+        <v>44.1</v>
+      </c>
+      <c r="D5" s="13">
+        <v>0.325</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5">
+      <c r="B6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="13">
+        <v>58.12</v>
+      </c>
+      <c r="D6" s="13">
+        <v>0.325</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5">
+      <c r="B7" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="13">
+        <v>72.15</v>
+      </c>
+      <c r="D7" s="13">
+        <v>0.325</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5">
+      <c r="B8" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="13">
+        <v>86.18</v>
+      </c>
+      <c r="D8" s="13">
+        <v>0.325</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5">
+      <c r="B9" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="13">
+        <v>100.2</v>
+      </c>
+      <c r="D9" s="13">
+        <v>0.325</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5">
+      <c r="B10" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="13">
+        <v>114.23</v>
+      </c>
+      <c r="D10" s="13">
+        <v>0.325</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5">
+      <c r="B11" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="13">
+        <v>128.26</v>
+      </c>
+      <c r="D11" s="13">
+        <v>0.325</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5">
+      <c r="B12" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="13">
+        <v>142.29</v>
+      </c>
+      <c r="D12" s="13">
+        <v>0.325</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5">
+      <c r="B13" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="13">
+        <v>156.31</v>
+      </c>
+      <c r="D13" s="13">
+        <v>0.325</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5">
+      <c r="B14" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="13">
+        <v>170.34</v>
+      </c>
+      <c r="D14" s="13">
+        <v>0.325</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5">
+      <c r="B15" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="13">
+        <v>184.37</v>
+      </c>
+      <c r="D15" s="13">
+        <v>0.325</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5">
+      <c r="B16" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="13">
+        <v>198.39</v>
+      </c>
+      <c r="D16" s="13">
+        <v>0.325</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5">
+      <c r="B17" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="13">
+        <v>212.42</v>
+      </c>
+      <c r="D17" s="13">
+        <v>0.325</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5">
+      <c r="B18" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="13">
+        <v>226.45</v>
+      </c>
+      <c r="D18" s="13">
+        <v>0.325</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5">
+      <c r="B19" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="13">
+        <v>240.48</v>
+      </c>
+      <c r="D19" s="13">
+        <v>0.325</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5">
+      <c r="B20" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="13">
+        <v>254.5</v>
+      </c>
+      <c r="D20" s="13">
+        <v>0.325</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.70" right="0.70" top="0.75" bottom="0.75" header="0.30" footer="0.30"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
FEAT: add reactor sheet
</commit_message>
<xml_diff>
--- a/input/Material/MaterialData.xlsx
+++ b/input/Material/MaterialData.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="Polaris Office Sheet" lastEdited="4" lowestEdited="4" rupBuild=""/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="25755" windowHeight="11595" activeTab="0"/>
+    <workbookView xWindow="360" yWindow="30" windowWidth="25755" windowHeight="11595" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="1" r:id="rId1"/>
     <sheet name="output" sheetId="2" r:id="rId2"/>
-    <sheet name="Example input data" sheetId="3" r:id="rId3"/>
-    <sheet name="Example output data" sheetId="4" r:id="rId4"/>
+    <sheet name="Reactor" sheetId="5" r:id="rId3"/>
+    <sheet name="Example input data" sheetId="3" r:id="rId4"/>
+    <sheet name="Example output data" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="152511"/>
@@ -18,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
   <si>
     <t>Material_Name</t>
   </si>
@@ -282,6 +283,12 @@
 - 물질은 위에서부터 아래까지 빈칸없이 작성해주셔야 합니다. 
 - 
 - </t>
+  </si>
+  <si>
+    <t>Reactor Name</t>
+  </si>
+  <si>
+    <t>Equipment Cost</t>
   </si>
 </sst>
 </file>
@@ -622,7 +629,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -851,12 +858,6 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top/>
-      <bottom/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color rgb="FFAAAAAA"/>
       </right>
@@ -1167,6 +1168,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1179,9 +1183,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1194,6 +1195,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1206,9 +1210,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1221,6 +1222,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1231,9 +1235,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2322,7 +2323,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Y40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="F2" sqref="F2:N13"/>
     </sheetView>
   </sheetViews>
@@ -3474,7 +3475,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:N20"/>
+  <dimension ref="B2:N20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E36" sqref="E36"/>
@@ -3886,6 +3887,35 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B2:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.200000"/>
+  <cols>
+    <col min="2" max="2" width="19.87999916" customWidth="1" outlineLevel="0"/>
+    <col min="3" max="3" width="20.75499916" customWidth="1" outlineLevel="0"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3">
+      <c r="B2" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>79</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.70" right="0.70" top="0.75" bottom="0.75" header="0.30" footer="0.30"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:D6"/>
   <sheetViews>
@@ -3962,7 +3992,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:E20"/>
   <sheetViews>

</xml_diff>

<commit_message>
FEAT: calc AtomicWeight by parse
</commit_message>
<xml_diff>
--- a/input/Material/MaterialData.xlsx
+++ b/input/Material/MaterialData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="Polaris Office Sheet" lastEdited="4" lowestEdited="4" rupBuild=""/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="25755" windowHeight="11595" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="30" windowWidth="25755" windowHeight="11595" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="1" r:id="rId1"/>
@@ -2221,7 +2221,7 @@
   <dimension ref="A1:Y40"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:N13"/>
+      <selection activeCell="D2" sqref="D2:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333000" defaultRowHeight="15.000000" customHeight="1"/>
@@ -2266,11 +2266,9 @@
         <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="D2" s="3"/>
       <c r="E2" s="1"/>
       <c r="F2" s="63" t="s">
         <v>37</v>
@@ -2301,11 +2299,9 @@
         <v>8</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="D3" s="3"/>
       <c r="E3" s="1"/>
       <c r="F3" s="66"/>
       <c r="N3" s="67"/>
@@ -2327,11 +2323,9 @@
         <v>11</v>
       </c>
       <c r="C4" s="9">
-        <v>2.016</v>
-      </c>
-      <c r="D4" s="9">
         <v>5</v>
       </c>
+      <c r="D4" s="9"/>
       <c r="E4" s="1"/>
       <c r="F4" s="66"/>
       <c r="N4" s="67"/>
@@ -2353,11 +2347,9 @@
         <v>12</v>
       </c>
       <c r="C5" s="9">
-        <v>32</v>
-      </c>
-      <c r="D5" s="9">
         <v>0.08</v>
       </c>
+      <c r="D5" s="9"/>
       <c r="E5" s="1"/>
       <c r="F5" s="66"/>
       <c r="N5" s="67"/>
@@ -2379,11 +2371,9 @@
         <v>13</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="6" t="s">
         <v>15</v>
       </c>
+      <c r="D6" s="6"/>
       <c r="E6" s="1"/>
       <c r="F6" s="66"/>
       <c r="N6" s="67"/>
@@ -3290,10 +3280,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:N20"/>
+  <dimension ref="B1:N20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.200000"/>
@@ -3309,12 +3299,9 @@
         <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>16</v>
       </c>
     </row>
@@ -3323,12 +3310,9 @@
         <v>17</v>
       </c>
       <c r="C3" s="10">
-        <v>16.04</v>
-      </c>
-      <c r="D3" s="10">
         <v>0.325</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="D3" s="0" t="s">
         <v>18</v>
       </c>
       <c r="F3" s="71" t="s">
@@ -3348,12 +3332,9 @@
         <v>20</v>
       </c>
       <c r="C4" s="10">
-        <v>30.07</v>
-      </c>
-      <c r="D4" s="10">
         <v>0.325</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="D4" s="0" t="s">
         <v>18</v>
       </c>
       <c r="F4" s="74"/>
@@ -3371,12 +3352,9 @@
         <v>21</v>
       </c>
       <c r="C5" s="10">
-        <v>44.1</v>
-      </c>
-      <c r="D5" s="10">
         <v>0.325</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="D5" s="0" t="s">
         <v>18</v>
       </c>
       <c r="F5" s="74"/>
@@ -3394,12 +3372,9 @@
         <v>22</v>
       </c>
       <c r="C6" s="10">
-        <v>58.12</v>
-      </c>
-      <c r="D6" s="10">
         <v>0.325</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="D6" s="0" t="s">
         <v>18</v>
       </c>
       <c r="F6" s="74"/>
@@ -3417,12 +3392,9 @@
         <v>23</v>
       </c>
       <c r="C7" s="10">
-        <v>72.15</v>
-      </c>
-      <c r="D7" s="10">
         <v>0.325</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="D7" s="0" t="s">
         <v>18</v>
       </c>
       <c r="F7" s="74"/>
@@ -3440,12 +3412,9 @@
         <v>24</v>
       </c>
       <c r="C8" s="10">
-        <v>86.18</v>
-      </c>
-      <c r="D8" s="10">
         <v>0.325</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="D8" s="0" t="s">
         <v>18</v>
       </c>
       <c r="F8" s="74"/>
@@ -3463,12 +3432,9 @@
         <v>25</v>
       </c>
       <c r="C9" s="10">
-        <v>100.2</v>
-      </c>
-      <c r="D9" s="10">
         <v>0.325</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="D9" s="0" t="s">
         <v>18</v>
       </c>
       <c r="F9" s="74"/>
@@ -3486,12 +3452,9 @@
         <v>26</v>
       </c>
       <c r="C10" s="10">
-        <v>114.23</v>
-      </c>
-      <c r="D10" s="10">
         <v>0.325</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="D10" s="0" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="74"/>
@@ -3509,12 +3472,9 @@
         <v>27</v>
       </c>
       <c r="C11" s="10">
-        <v>128.26</v>
-      </c>
-      <c r="D11" s="10">
         <v>0.325</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="D11" s="0" t="s">
         <v>18</v>
       </c>
       <c r="F11" s="74"/>
@@ -3532,12 +3492,9 @@
         <v>28</v>
       </c>
       <c r="C12" s="10">
-        <v>142.29</v>
-      </c>
-      <c r="D12" s="10">
         <v>0.325</v>
       </c>
-      <c r="E12" s="0" t="s">
+      <c r="D12" s="0" t="s">
         <v>18</v>
       </c>
       <c r="F12" s="74"/>
@@ -3555,12 +3512,9 @@
         <v>29</v>
       </c>
       <c r="C13" s="10">
-        <v>156.31</v>
-      </c>
-      <c r="D13" s="10">
         <v>0.325</v>
       </c>
-      <c r="E13" s="0" t="s">
+      <c r="D13" s="0" t="s">
         <v>18</v>
       </c>
       <c r="F13" s="74"/>
@@ -3578,12 +3532,9 @@
         <v>30</v>
       </c>
       <c r="C14" s="10">
-        <v>170.34</v>
-      </c>
-      <c r="D14" s="10">
         <v>0.325</v>
       </c>
-      <c r="E14" s="0" t="s">
+      <c r="D14" s="0" t="s">
         <v>18</v>
       </c>
       <c r="F14" s="74"/>
@@ -3601,12 +3552,9 @@
         <v>31</v>
       </c>
       <c r="C15" s="10">
-        <v>184.37</v>
-      </c>
-      <c r="D15" s="10">
         <v>0.325</v>
       </c>
-      <c r="E15" s="0" t="s">
+      <c r="D15" s="0" t="s">
         <v>18</v>
       </c>
       <c r="F15" s="77"/>
@@ -3624,12 +3572,9 @@
         <v>32</v>
       </c>
       <c r="C16" s="10">
-        <v>198.39</v>
-      </c>
-      <c r="D16" s="10">
         <v>0.325</v>
       </c>
-      <c r="E16" s="0" t="s">
+      <c r="D16" s="0" t="s">
         <v>18</v>
       </c>
     </row>
@@ -3638,12 +3583,9 @@
         <v>33</v>
       </c>
       <c r="C17" s="10">
-        <v>212.42</v>
-      </c>
-      <c r="D17" s="10">
         <v>0.325</v>
       </c>
-      <c r="E17" s="0" t="s">
+      <c r="D17" s="0" t="s">
         <v>18</v>
       </c>
     </row>
@@ -3652,12 +3594,9 @@
         <v>34</v>
       </c>
       <c r="C18" s="10">
-        <v>226.45</v>
-      </c>
-      <c r="D18" s="10">
         <v>0.325</v>
       </c>
-      <c r="E18" s="0" t="s">
+      <c r="D18" s="0" t="s">
         <v>18</v>
       </c>
       <c r="G18" s="12"/>
@@ -3667,12 +3606,9 @@
         <v>35</v>
       </c>
       <c r="C19" s="10">
-        <v>240.48</v>
-      </c>
-      <c r="D19" s="10">
         <v>0.325</v>
       </c>
-      <c r="E19" s="0" t="s">
+      <c r="D19" s="0" t="s">
         <v>18</v>
       </c>
     </row>
@@ -3681,12 +3617,9 @@
         <v>36</v>
       </c>
       <c r="C20" s="10">
-        <v>254.5</v>
-      </c>
-      <c r="D20" s="10">
         <v>0.325</v>
       </c>
-      <c r="E20" s="0" t="s">
+      <c r="D20" s="0" t="s">
         <v>18</v>
       </c>
     </row>
@@ -3704,7 +3637,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -3726,15 +3659,24 @@
       <c r="B3" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="C3" s="0">
+        <v>123</v>
+      </c>
     </row>
     <row r="4" spans="2:3">
       <c r="B4" s="0" t="s">
         <v>3</v>
       </c>
+      <c r="C4" s="0">
+        <v>123</v>
+      </c>
     </row>
     <row r="5" spans="2:3">
       <c r="B5" s="0" t="s">
         <v>4</v>
+      </c>
+      <c r="C5" s="0">
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Style : change manual
</commit_message>
<xml_diff>
--- a/input/Material/MaterialData.xlsx
+++ b/input/Material/MaterialData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="Polaris Office Sheet" lastEdited="4" lowestEdited="4" rupBuild=""/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="25755" windowHeight="11595" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="30" windowWidth="25755" windowHeight="11595" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Reactor Name</t>
   </si>
@@ -143,6 +143,12 @@
 - 물질은 위에서부터 아래까지 빈칸없이 작성해주셔야 합니다. 
 - 
 - </t>
+  </si>
+  <si>
+    <t>Natural Gas2</t>
+  </si>
+  <si>
+    <t>Natural Gas 2</t>
   </si>
 </sst>
 </file>
@@ -2221,7 +2227,7 @@
   <dimension ref="A1:Y40"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D6"/>
+      <selection activeCell="F2" sqref="F2:N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333000" defaultRowHeight="15.000000" customHeight="1"/>
@@ -3280,10 +3286,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:N20"/>
+  <dimension ref="B2:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.200000"/>
@@ -3555,7 +3561,7 @@
         <v>0.325</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="F15" s="77"/>
       <c r="G15" s="78"/>
@@ -3575,7 +3581,7 @@
         <v>0.325</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="2:7">
@@ -3691,7 +3697,7 @@
   <dimension ref="B2:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D2" sqref="D2:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.200000"/>
@@ -3706,55 +3712,45 @@
         <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="D2" s="3"/>
     </row>
     <row r="3" spans="2:4">
       <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="D3" s="3"/>
     </row>
     <row r="4" spans="2:4">
       <c r="B4" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="9">
-        <v>2.016</v>
-      </c>
-      <c r="D4" s="9">
         <v>5</v>
       </c>
+      <c r="D4" s="9"/>
     </row>
     <row r="5" spans="2:4">
       <c r="B5" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="9">
-        <v>32</v>
-      </c>
-      <c r="D5" s="9">
         <v>0.08</v>
       </c>
+      <c r="D5" s="9"/>
     </row>
     <row r="6" spans="2:4">
       <c r="B6" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="6" t="s">
         <v>15</v>
       </c>
+      <c r="D6" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -3765,10 +3761,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:E20"/>
+  <dimension ref="B1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.200000"/>
@@ -3779,269 +3775,212 @@
     <col min="5" max="5" width="12.13000011" customWidth="1" outlineLevel="0"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5">
+    <row r="2" spans="2:4">
       <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="2:5">
+    <row r="3" spans="2:4">
       <c r="B3" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="10">
-        <v>16.04</v>
-      </c>
-      <c r="D3" s="10">
         <v>0.325</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="D3" s="0" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="2:5">
+    <row r="4" spans="2:4">
       <c r="B4" s="6" t="s">
         <v>20</v>
       </c>
       <c r="C4" s="10">
-        <v>30.07</v>
-      </c>
-      <c r="D4" s="10">
         <v>0.325</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="D4" s="0" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="2:5">
+    <row r="5" spans="2:4">
       <c r="B5" s="6" t="s">
         <v>21</v>
       </c>
       <c r="C5" s="10">
-        <v>44.1</v>
-      </c>
-      <c r="D5" s="10">
         <v>0.325</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="D5" s="0" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="2:5">
+    <row r="6" spans="2:4">
       <c r="B6" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C6" s="10">
-        <v>58.12</v>
-      </c>
-      <c r="D6" s="10">
         <v>0.325</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="D6" s="0" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="2:5">
+    <row r="7" spans="2:4">
       <c r="B7" s="6" t="s">
         <v>23</v>
       </c>
       <c r="C7" s="10">
-        <v>72.15</v>
-      </c>
-      <c r="D7" s="10">
         <v>0.325</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="D7" s="0" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="2:5">
+    <row r="8" spans="2:4">
       <c r="B8" s="6" t="s">
         <v>24</v>
       </c>
       <c r="C8" s="10">
-        <v>86.18</v>
-      </c>
-      <c r="D8" s="10">
         <v>0.325</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="D8" s="0" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="2:5">
+    <row r="9" spans="2:4">
       <c r="B9" s="6" t="s">
         <v>25</v>
       </c>
       <c r="C9" s="10">
-        <v>100.2</v>
-      </c>
-      <c r="D9" s="10">
         <v>0.325</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="D9" s="0" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="2:5">
+    <row r="10" spans="2:4">
       <c r="B10" s="6" t="s">
         <v>26</v>
       </c>
       <c r="C10" s="10">
-        <v>114.23</v>
-      </c>
-      <c r="D10" s="10">
         <v>0.325</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="D10" s="0" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="2:5">
+    <row r="11" spans="2:4">
       <c r="B11" s="6" t="s">
         <v>27</v>
       </c>
       <c r="C11" s="10">
-        <v>128.26</v>
-      </c>
-      <c r="D11" s="10">
         <v>0.325</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="D11" s="0" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="2:5">
+    <row r="12" spans="2:4">
       <c r="B12" s="6" t="s">
         <v>28</v>
       </c>
       <c r="C12" s="10">
-        <v>142.29</v>
-      </c>
-      <c r="D12" s="10">
         <v>0.325</v>
       </c>
-      <c r="E12" s="0" t="s">
+      <c r="D12" s="0" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="2:5">
+    <row r="13" spans="2:4">
       <c r="B13" s="6" t="s">
         <v>29</v>
       </c>
       <c r="C13" s="10">
-        <v>156.31</v>
-      </c>
-      <c r="D13" s="10">
         <v>0.325</v>
       </c>
-      <c r="E13" s="0" t="s">
+      <c r="D13" s="0" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="2:5">
+    <row r="14" spans="2:4">
       <c r="B14" s="6" t="s">
         <v>30</v>
       </c>
       <c r="C14" s="10">
-        <v>170.34</v>
-      </c>
-      <c r="D14" s="10">
         <v>0.325</v>
       </c>
-      <c r="E14" s="0" t="s">
+      <c r="D14" s="0" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="2:5">
+    <row r="15" spans="2:4">
       <c r="B15" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C15" s="10">
-        <v>184.37</v>
-      </c>
-      <c r="D15" s="10">
         <v>0.325</v>
       </c>
-      <c r="E15" s="0" t="s">
+      <c r="D15" s="0" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="2:5">
+    <row r="16" spans="2:4">
       <c r="B16" s="6" t="s">
         <v>32</v>
       </c>
       <c r="C16" s="10">
-        <v>198.39</v>
-      </c>
-      <c r="D16" s="10">
         <v>0.325</v>
       </c>
-      <c r="E16" s="0" t="s">
+      <c r="D16" s="0" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="2:5">
+    <row r="17" spans="2:4">
       <c r="B17" s="6" t="s">
         <v>33</v>
       </c>
       <c r="C17" s="10">
-        <v>212.42</v>
-      </c>
-      <c r="D17" s="10">
         <v>0.325</v>
       </c>
-      <c r="E17" s="0" t="s">
+      <c r="D17" s="0" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="2:5">
+    <row r="18" spans="2:4">
       <c r="B18" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C18" s="10">
-        <v>226.45</v>
-      </c>
-      <c r="D18" s="10">
         <v>0.325</v>
       </c>
-      <c r="E18" s="0" t="s">
+      <c r="D18" s="0" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="2:5">
+    <row r="19" spans="2:4">
       <c r="B19" s="6" t="s">
         <v>35</v>
       </c>
       <c r="C19" s="10">
-        <v>240.48</v>
-      </c>
-      <c r="D19" s="10">
         <v>0.325</v>
       </c>
-      <c r="E19" s="0" t="s">
+      <c r="D19" s="0" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="2:5">
+    <row r="20" spans="2:4">
       <c r="B20" s="6" t="s">
         <v>36</v>
       </c>
       <c r="C20" s="10">
-        <v>254.5</v>
-      </c>
-      <c r="D20" s="10">
         <v>0.325</v>
       </c>
-      <c r="E20" s="0" t="s">
+      <c r="D20" s="0" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Feat: parse param in Excel and change autofit
</commit_message>
<xml_diff>
--- a/input/Material/MaterialData.xlsx
+++ b/input/Material/MaterialData.xlsx
@@ -10,8 +10,10 @@
     <sheet name="input" sheetId="1" r:id="rId1"/>
     <sheet name="output" sheetId="2" r:id="rId2"/>
     <sheet name="Reactor" sheetId="3" r:id="rId3"/>
-    <sheet name="Example input data" sheetId="4" r:id="rId4"/>
-    <sheet name="Example output data" sheetId="5" r:id="rId5"/>
+    <sheet name="Equipment Cost Parameter" sheetId="6" r:id="rId4"/>
+    <sheet name="Utility Parameter" sheetId="7" r:id="rId5"/>
+    <sheet name="Example input data" sheetId="4" r:id="rId6"/>
+    <sheet name="Example output data" sheetId="5" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="152511"/>
@@ -19,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
   <si>
     <t>Reactor Name</t>
   </si>
@@ -39,18 +41,12 @@
     <t>Material_Name</t>
   </si>
   <si>
-    <t>Material_Weight [g/mol]</t>
-  </si>
-  <si>
     <t>Material_Cost [USD/kg]</t>
   </si>
   <si>
     <t>CO2</t>
   </si>
   <si>
-    <t>44.01</t>
-  </si>
-  <si>
     <t>0.0558</t>
   </si>
   <si>
@@ -61,9 +57,6 @@
   </si>
   <si>
     <t>H2O</t>
-  </si>
-  <si>
-    <t>18.015</t>
   </si>
   <si>
     <t>0.00053</t>
@@ -122,6 +115,9 @@
     <t>C13H28</t>
   </si>
   <si>
+    <t>Natural Gas 2</t>
+  </si>
+  <si>
     <t>C14H30</t>
   </si>
   <si>
@@ -145,10 +141,137 @@
 - </t>
   </si>
   <si>
-    <t>Natural Gas2</t>
-  </si>
-  <si>
-    <t>Natural Gas 2</t>
+    <t>Heater</t>
+  </si>
+  <si>
+    <t>HEATER</t>
+  </si>
+  <si>
+    <t>Diphenyl heater</t>
+  </si>
+  <si>
+    <t>Molten salt heater</t>
+  </si>
+  <si>
+    <t>Hot water heater</t>
+  </si>
+  <si>
+    <t>Steam boiler</t>
+  </si>
+  <si>
+    <t>HeatExchanger</t>
+  </si>
+  <si>
+    <t>Fixed tube</t>
+  </si>
+  <si>
+    <t>Floating head</t>
+  </si>
+  <si>
+    <t>U-tube</t>
+  </si>
+  <si>
+    <t>Bayonet</t>
+  </si>
+  <si>
+    <t>ompressor</t>
+  </si>
+  <si>
+    <t>Compressor</t>
+  </si>
+  <si>
+    <t>Centrifugal, axial and reciprocating</t>
+  </si>
+  <si>
+    <t>Rotary</t>
+  </si>
+  <si>
+    <t>K1</t>
+  </si>
+  <si>
+    <t>K2</t>
+  </si>
+  <si>
+    <t>K3</t>
+  </si>
+  <si>
+    <t>"Diphenyl heater" : {"K1": 2.2628, "K2": 0.8581, "K3": 0.0003} ,
+	"Molten salt heater" : {"K1": 1.1979, "K2": 1.4782, "K3": -0.0958} ,
+	"Hot water heater" : {"K1": 2.0829, "K2": 0.9074, "K3": -0.0243} ,
+	"Steam boiler" : {"K1": 6.9617, "K2": -1.48, "K3": 0.3161}</t>
+  </si>
+  <si>
+    <t>"Fixed tube" : {"K1": 4.3247, "K2": -0.303, "K3": 0.1634},
+	"Floating head" : {"K1": 4.8306, "K2": -0.8509, "K3": 0.3187},
+	"U-tube" : {"K1": 4.1884, "K2": -0.2503, "K3": 0.1974},
+	"Bayonet" : {"K1": 4.2768, "K2": -0.0495, "K3": 0.1431}</t>
+  </si>
+  <si>
+    <t>"Centrifugal, axial and reciprocating" : {"K1": 2.2891, "K2": 1.3604, "K3": -0.1027},
+	"Rotary" : {"K1": 5.0355, "K2": -1.8002, "K3": 0.8253}</t>
+  </si>
+  <si>
+    <t>utilityCostData</t>
+  </si>
+  <si>
+    <t>calcOPEXdata</t>
+  </si>
+  <si>
+    <t>profitAnalysisData</t>
+  </si>
+  <si>
+    <t>electricityCostPerKWH</t>
+  </si>
+  <si>
+    <t>NGprice</t>
+  </si>
+  <si>
+    <t>CoolingWaterPrice</t>
+  </si>
+  <si>
+    <t>coolingWaterPrice</t>
+  </si>
+  <si>
+    <t>catalystPrice</t>
+  </si>
+  <si>
+    <t>plantOperationHours</t>
+  </si>
+  <si>
+    <t>depreciationLifetime</t>
+  </si>
+  <si>
+    <t>USD/kg</t>
+  </si>
+  <si>
+    <t>USD/kWh</t>
+  </si>
+  <si>
+    <t>USD/ton</t>
+  </si>
+  <si>
+    <t>#hours/year</t>
+  </si>
+  <si>
+    <t>years</t>
+  </si>
+  <si>
+    <t>hours/year</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Fired heater Natural gas price</t>
+  </si>
+  <si>
+    <t>ELECTRICITY UTILITY 계산할 때 사용</t>
+  </si>
+  <si>
+    <t>Cooling utility 계산할 때 사용</t>
   </si>
 </sst>
 </file>
@@ -156,7 +279,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="23">
+  <fonts count="38">
     <font>
       <sz val="11.0"/>
       <name val="나눔스퀘어"/>
@@ -278,6 +401,86 @@
     <font>
       <sz val="12.0"/>
       <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="9.0"/>
+      <name val="Menlo"/>
+      <color rgb="FF9CDCFE"/>
+    </font>
+    <font>
+      <sz val="9.0"/>
+      <name val="Menlo"/>
+      <color theme="1"/>
+    </font>
+    <font>
+      <sz val="9.0"/>
+      <name val="Menlo"/>
+      <color rgb="FFCE9178"/>
+    </font>
+    <font>
+      <sz val="9.0"/>
+      <name val="Menlo"/>
+      <color rgb="FF000000"/>
+    </font>
+    <font>
+      <sz val="10.0"/>
+      <name val="Menlo"/>
+      <color theme="1"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="Menlo"/>
+      <color theme="1"/>
+    </font>
+    <font>
+      <sz val="10.0"/>
+      <name val="Menlo"/>
+      <color rgb="FF000000"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="Menlo"/>
+      <color rgb="FF000000"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.0"/>
+      <name val="Menlo"/>
+      <color rgb="FF000000"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.0"/>
+      <name val="Menlo"/>
+      <color theme="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.0"/>
+      <name val="나눔스퀘어"/>
+      <color rgb="FF000000"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9.0"/>
+      <name val="Menlo"/>
+      <color rgb="FF000000"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10.0"/>
+      <name val="Menlo"/>
+      <color rgb="FF000000"/>
+    </font>
+    <font>
+      <sz val="9.0"/>
+      <name val="Menlo"/>
+      <color rgb="FF6A9955"/>
+    </font>
+    <font>
+      <sz val="9.0"/>
+      <name val="Menlo"/>
+      <color rgb="FFB5CEA8"/>
     </font>
   </fonts>
   <fills count="35">
@@ -916,7 +1119,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0"/>
@@ -1143,6 +1346,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="20% - 강조색1" xfId="25" builtinId="30"/>
@@ -2272,12 +2503,12 @@
         <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="1"/>
       <c r="F2" s="63" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G2" s="64"/>
       <c r="H2" s="64"/>
@@ -2302,10 +2533,10 @@
     <row r="3" spans="1:25" ht="16.000000" customHeight="1">
       <c r="A3" s="1"/>
       <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>10</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="1"/>
@@ -2326,7 +2557,7 @@
     <row r="4" spans="1:25" ht="16.000000" customHeight="1">
       <c r="A4" s="1"/>
       <c r="B4" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C4" s="9">
         <v>5</v>
@@ -2350,7 +2581,7 @@
     <row r="5" spans="1:25" ht="16.000000" customHeight="1">
       <c r="A5" s="1"/>
       <c r="B5" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C5" s="9">
         <v>0.08</v>
@@ -2374,10 +2605,10 @@
     <row r="6" spans="1:25" ht="16.000000" customHeight="1">
       <c r="A6" s="1"/>
       <c r="B6" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="1"/>
@@ -3305,24 +3536,24 @@
         <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="2:14">
       <c r="B3" s="6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C3" s="10">
         <v>0.325</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F3" s="71" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G3" s="72"/>
       <c r="H3" s="72"/>
@@ -3335,13 +3566,13 @@
     </row>
     <row r="4" spans="2:14">
       <c r="B4" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C4" s="10">
         <v>0.325</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F4" s="74"/>
       <c r="G4" s="75"/>
@@ -3355,13 +3586,13 @@
     </row>
     <row r="5" spans="2:14">
       <c r="B5" s="6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C5" s="10">
         <v>0.325</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F5" s="74"/>
       <c r="G5" s="75"/>
@@ -3375,13 +3606,13 @@
     </row>
     <row r="6" spans="2:14">
       <c r="B6" s="6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C6" s="10">
         <v>0.325</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F6" s="74"/>
       <c r="G6" s="75"/>
@@ -3395,13 +3626,13 @@
     </row>
     <row r="7" spans="2:14">
       <c r="B7" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C7" s="10">
         <v>0.325</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F7" s="74"/>
       <c r="G7" s="75"/>
@@ -3415,13 +3646,13 @@
     </row>
     <row r="8" spans="2:14">
       <c r="B8" s="6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C8" s="10">
         <v>0.325</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F8" s="74"/>
       <c r="G8" s="75"/>
@@ -3435,13 +3666,13 @@
     </row>
     <row r="9" spans="2:14">
       <c r="B9" s="6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C9" s="10">
         <v>0.325</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F9" s="74"/>
       <c r="G9" s="75"/>
@@ -3455,13 +3686,13 @@
     </row>
     <row r="10" spans="2:14">
       <c r="B10" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C10" s="10">
         <v>0.325</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F10" s="74"/>
       <c r="G10" s="75"/>
@@ -3475,13 +3706,13 @@
     </row>
     <row r="11" spans="2:14">
       <c r="B11" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C11" s="10">
         <v>0.325</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F11" s="74"/>
       <c r="G11" s="75"/>
@@ -3495,13 +3726,13 @@
     </row>
     <row r="12" spans="2:14">
       <c r="B12" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C12" s="10">
         <v>0.325</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F12" s="74"/>
       <c r="G12" s="75"/>
@@ -3515,13 +3746,13 @@
     </row>
     <row r="13" spans="2:14">
       <c r="B13" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C13" s="10">
         <v>0.325</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F13" s="74"/>
       <c r="G13" s="75"/>
@@ -3535,13 +3766,13 @@
     </row>
     <row r="14" spans="2:14">
       <c r="B14" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C14" s="10">
         <v>0.325</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F14" s="74"/>
       <c r="G14" s="75"/>
@@ -3555,13 +3786,13 @@
     </row>
     <row r="15" spans="2:14">
       <c r="B15" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C15" s="10">
         <v>0.325</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="F15" s="77"/>
       <c r="G15" s="78"/>
@@ -3575,58 +3806,58 @@
     </row>
     <row r="16" spans="2:14">
       <c r="B16" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C16" s="10">
         <v>0.325</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="2:7">
       <c r="B17" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C17" s="10">
         <v>0.325</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="2:7">
       <c r="B18" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C18" s="10">
         <v>0.325</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G18" s="12"/>
     </row>
     <row r="19" spans="2:7">
       <c r="B19" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C19" s="10">
         <v>0.325</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="2:7">
       <c r="B20" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C20" s="10">
         <v>0.325</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -3644,7 +3875,7 @@
   <dimension ref="B2:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.200000"/>
@@ -3674,7 +3905,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="0">
-        <v>123</v>
+        <v>2222</v>
       </c>
     </row>
     <row r="5" spans="2:3">
@@ -3682,7 +3913,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="0">
-        <v>123</v>
+        <v>123123</v>
       </c>
     </row>
   </sheetData>
@@ -3693,6 +3924,399 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B2:K18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.200000"/>
+  <cols>
+    <col min="2" max="2" width="35.38000107" customWidth="1" outlineLevel="0"/>
+    <col min="3" max="3" width="11.25500011" customWidth="1" outlineLevel="0"/>
+    <col min="4" max="4" width="11.75500011" customWidth="1" outlineLevel="0"/>
+    <col min="5" max="5" width="10.63000011" customWidth="1" outlineLevel="0"/>
+    <col min="7" max="7" width="9.50500011" customWidth="1" outlineLevel="0"/>
+    <col min="11" max="11" width="74.75499725" customWidth="1" outlineLevel="0"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:11">
+      <c r="B2" s="90" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="91" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="91" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="91" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" s="94"/>
+      <c r="I2" s="95"/>
+      <c r="J2" s="95"/>
+      <c r="K2" s="95"/>
+    </row>
+    <row r="3" spans="2:11">
+      <c r="B3" s="83" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="0">
+        <v>2.2628</v>
+      </c>
+      <c r="D3" s="0">
+        <v>0.8581</v>
+      </c>
+      <c r="E3" s="0">
+        <v>3E-04</v>
+      </c>
+      <c r="H3" s="95"/>
+      <c r="I3" s="95"/>
+      <c r="J3" s="95"/>
+      <c r="K3" s="95"/>
+    </row>
+    <row r="4" spans="2:11">
+      <c r="B4" s="83" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="0">
+        <v>1.1979</v>
+      </c>
+      <c r="D4" s="0">
+        <v>1.4782</v>
+      </c>
+      <c r="E4" s="0">
+        <v>-0.0958</v>
+      </c>
+      <c r="H4" s="95"/>
+      <c r="I4" s="95"/>
+      <c r="J4" s="95"/>
+      <c r="K4" s="95"/>
+    </row>
+    <row r="5" spans="2:11">
+      <c r="B5" s="83" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="0">
+        <v>2.0829</v>
+      </c>
+      <c r="D5" s="0">
+        <v>0.9074</v>
+      </c>
+      <c r="E5" s="0">
+        <v>-0.0243</v>
+      </c>
+      <c r="H5" s="95"/>
+      <c r="I5" s="95"/>
+      <c r="J5" s="95"/>
+      <c r="K5" s="95"/>
+    </row>
+    <row r="6" spans="2:11">
+      <c r="B6" s="83" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="0">
+        <v>6.9617</v>
+      </c>
+      <c r="D6" s="0">
+        <v>-1.48</v>
+      </c>
+      <c r="E6" s="0">
+        <v>0.3161</v>
+      </c>
+      <c r="H6" s="95"/>
+      <c r="I6" s="95"/>
+      <c r="J6" s="95"/>
+      <c r="K6" s="95"/>
+    </row>
+    <row r="7" spans="2:11">
+      <c r="B7" s="84"/>
+      <c r="H7" s="95"/>
+      <c r="I7" s="95"/>
+      <c r="J7" s="95"/>
+      <c r="K7" s="95"/>
+    </row>
+    <row r="8" spans="2:11">
+      <c r="B8" s="84"/>
+      <c r="H8" s="95"/>
+      <c r="I8" s="95"/>
+      <c r="J8" s="95"/>
+      <c r="K8" s="95"/>
+    </row>
+    <row r="9" spans="2:11">
+      <c r="B9" s="89" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="91" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="91" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="91" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11">
+      <c r="B10" s="83" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="0">
+        <v>4.3247</v>
+      </c>
+      <c r="D10" s="0">
+        <v>-0.303</v>
+      </c>
+      <c r="E10" s="0">
+        <v>0.1634</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11">
+      <c r="B11" s="83" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="0">
+        <v>4.8306</v>
+      </c>
+      <c r="D11" s="0">
+        <v>-0.8509</v>
+      </c>
+      <c r="E11" s="0">
+        <v>0.3187</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11">
+      <c r="B12" s="83" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="0">
+        <v>4.1884</v>
+      </c>
+      <c r="D12" s="0">
+        <v>-0.2503</v>
+      </c>
+      <c r="E12" s="0">
+        <v>0.1974</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11">
+      <c r="B13" s="83" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="0">
+        <v>4.2768</v>
+      </c>
+      <c r="D13" s="0">
+        <v>-0.0495</v>
+      </c>
+      <c r="E13" s="0">
+        <v>0.1431</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11">
+      <c r="B14" s="84"/>
+    </row>
+    <row r="15" spans="2:11">
+      <c r="B15" s="84"/>
+    </row>
+    <row r="16" spans="2:11">
+      <c r="B16" s="89" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="91" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="91" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" s="91" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5">
+      <c r="B17" s="83" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="0">
+        <v>2.2891</v>
+      </c>
+      <c r="D17" s="0">
+        <v>1.3604</v>
+      </c>
+      <c r="E17" s="0">
+        <v>-0.1027</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5">
+      <c r="B18" s="83" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="0">
+        <v>5.0355</v>
+      </c>
+      <c r="D18" s="0">
+        <v>-1.8002</v>
+      </c>
+      <c r="E18" s="0">
+        <v>0.8253</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H2:K8"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.70" right="0.70" top="0.75" bottom="0.75" header="0.30" footer="0.30"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B2:AH15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.200000"/>
+  <cols>
+    <col min="2" max="2" width="33.88000107" customWidth="1" outlineLevel="0"/>
+    <col min="3" max="3" width="16.13000011" customWidth="1" outlineLevel="0"/>
+    <col min="4" max="4" width="13.88000011" customWidth="1" outlineLevel="0"/>
+    <col min="5" max="5" width="31.12999916" customWidth="1" outlineLevel="0"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:34">
+      <c r="B2" s="89" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="2:34">
+      <c r="B3" s="83" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="83">
+        <v>0.1088</v>
+      </c>
+      <c r="D3" s="83" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" s="98" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="2:34">
+      <c r="B4" s="83" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="83">
+        <v>0.0075</v>
+      </c>
+      <c r="D4" s="83" t="s">
+        <v>68</v>
+      </c>
+      <c r="E4" s="98" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="2:34">
+      <c r="B5" s="83" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="83">
+        <v>5.3E-04</v>
+      </c>
+      <c r="D5" s="83" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="98" t="s">
+        <v>77</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="2:34">
+      <c r="B6" s="84"/>
+      <c r="D6" s="84"/>
+      <c r="AH6" s="0" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="2:34">
+      <c r="B7" s="84"/>
+      <c r="D7" s="84"/>
+    </row>
+    <row r="8" spans="2:34">
+      <c r="B8" s="89" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="84"/>
+    </row>
+    <row r="9" spans="2:34">
+      <c r="B9" s="84" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="0">
+        <v>1</v>
+      </c>
+      <c r="D9" s="83" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="2:34">
+      <c r="B10" s="84" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="0">
+        <v>8400</v>
+      </c>
+      <c r="D10" s="83" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="2:34">
+      <c r="B11" s="84"/>
+      <c r="D11" s="84"/>
+    </row>
+    <row r="12" spans="2:34">
+      <c r="B12" s="84"/>
+      <c r="D12" s="84"/>
+    </row>
+    <row r="13" spans="2:34">
+      <c r="B13" s="89" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="84"/>
+    </row>
+    <row r="14" spans="2:34">
+      <c r="B14" s="84" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" s="0">
+        <v>20</v>
+      </c>
+      <c r="D14" s="83" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="2:34">
+      <c r="B15" s="84"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.70" right="0.70" top="0.75" bottom="0.75" header="0.30" footer="0.30"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:D6"/>
   <sheetViews>
@@ -3712,22 +4336,22 @@
         <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" s="3"/>
     </row>
     <row r="3" spans="2:4">
       <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>10</v>
       </c>
       <c r="D3" s="3"/>
     </row>
     <row r="4" spans="2:4">
       <c r="B4" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C4" s="9">
         <v>5</v>
@@ -3736,7 +4360,7 @@
     </row>
     <row r="5" spans="2:4">
       <c r="B5" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C5" s="9">
         <v>0.08</v>
@@ -3745,10 +4369,10 @@
     </row>
     <row r="6" spans="2:4">
       <c r="B6" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D6" s="6"/>
     </row>
@@ -3759,11 +4383,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:D20"/>
+  <dimension ref="B2:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2:E20"/>
     </sheetView>
   </sheetViews>
@@ -3780,208 +4404,208 @@
         <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="2:4">
       <c r="B3" s="6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C3" s="10">
         <v>0.325</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="2:4">
       <c r="B4" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C4" s="10">
         <v>0.325</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="2:4">
       <c r="B5" s="6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C5" s="10">
         <v>0.325</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="2:4">
       <c r="B6" s="6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C6" s="10">
         <v>0.325</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="2:4">
       <c r="B7" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C7" s="10">
         <v>0.325</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="2:4">
       <c r="B8" s="6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C8" s="10">
         <v>0.325</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="2:4">
       <c r="B9" s="6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C9" s="10">
         <v>0.325</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="2:4">
       <c r="B10" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C10" s="10">
         <v>0.325</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="2:4">
       <c r="B11" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C11" s="10">
         <v>0.325</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="2:4">
       <c r="B12" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C12" s="10">
         <v>0.325</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="2:4">
       <c r="B13" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C13" s="10">
         <v>0.325</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="2:4">
       <c r="B14" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C14" s="10">
         <v>0.325</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="2:4">
       <c r="B15" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C15" s="10">
         <v>0.325</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="2:4">
       <c r="B16" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C16" s="10">
         <v>0.325</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="2:4">
       <c r="B17" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C17" s="10">
         <v>0.325</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="2:4">
       <c r="B18" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C18" s="10">
         <v>0.325</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="2:4">
       <c r="B19" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C19" s="10">
         <v>0.325</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="2:4">
       <c r="B20" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C20" s="10">
         <v>0.325</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Style : add reactor cost unit
</commit_message>
<xml_diff>
--- a/input/Material/MaterialData.xlsx
+++ b/input/Material/MaterialData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="Polaris Office Sheet" lastEdited="4" lowestEdited="4" rupBuild=""/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="25755" windowHeight="11595" activeTab="4"/>
+    <workbookView xWindow="360" yWindow="30" windowWidth="25755" windowHeight="11595" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
   <si>
     <t>Reactor Name</t>
   </si>
@@ -272,6 +272,15 @@
   </si>
   <si>
     <t>Cooling utility 계산할 때 사용</t>
+  </si>
+  <si>
+    <t>[USD]</t>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>Equipment Cost[USD]</t>
   </si>
 </sst>
 </file>
@@ -3872,10 +3881,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:C5"/>
+  <dimension ref="B1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.200000"/>
@@ -3889,7 +3898,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>1</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="2:3">
@@ -4177,7 +4186,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:AH15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>

</xml_diff>